<commit_message>
intro to raster 01
</commit_message>
<xml_diff>
--- a/research_proj/annotated_lit_review.xlsx
+++ b/research_proj/annotated_lit_review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxzhang/GU/683GIS/research_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F613818-FE81-8E46-B4A9-4F247F56A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9041202C-3622-9041-86F3-B9E056657B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{81FDDBFB-4DC6-F243-9750-924FCF4562FA}"/>
   </bookViews>
@@ -435,23 +435,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -771,7 +771,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -788,11 +788,11 @@
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
@@ -829,7 +829,7 @@
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -849,7 +849,7 @@
       <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -869,7 +869,7 @@
       <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -889,7 +889,7 @@
       <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -909,7 +909,7 @@
       <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -929,7 +929,7 @@
       <c r="D8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -943,13 +943,13 @@
       <c r="B9" s="14">
         <v>2021</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -969,7 +969,7 @@
       <c r="D10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -983,13 +983,13 @@
       <c r="B11" s="14">
         <v>2013</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -1009,7 +1009,7 @@
       <c r="D12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="21" t="s">
         <v>51</v>
       </c>
       <c r="F12" s="11" t="s">

</xml_diff>